<commit_message>
Fixed target m/z values
</commit_message>
<xml_diff>
--- a/BASIC_DART-ExampleLibrary_Metadata.xlsx
+++ b/BASIC_DART-ExampleLibrary_Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/arunmoorthy_trentu_ca/Documents/RESEARCH/Projects/CRAFTS-DB_Builder/ForGithub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="14_{CF47B13E-3DF5-AA40-9E74-923CF73DCF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{547C9E55-983B-EB47-A472-52F251451B10}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="14_{CF47B13E-3DF5-AA40-9E74-923CF73DCF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFAE51AB-D9A5-9348-9C01-E20E0741FEF6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{FC49DEAF-D748-4197-AEBE-BC30185F4B2D}"/>
   </bookViews>
@@ -9695,7 +9695,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>322.2045</v>
+        <v>323.21230000000003</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -9706,7 +9706,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>135.10480000000001</v>
+        <v>136.11259999999999</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -9717,7 +9717,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>322.2045</v>
+        <v>323.21230000000003</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -9728,7 +9728,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>149.12039999999999</v>
+        <v>150.1283</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -14849,12 +14849,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EA0CA1719E747F44B1D00F49D3F6238C" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d928c6ceea87d3cf0155d6f895ca2634">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64be0a4d-3311-429d-90bd-b8f8a98a2612" xmlns:ns3="71fe8976-8fa5-4ae7-925c-3f33484c4e59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3aa75b4f87bfb021658e59fecd8c86ef" ns2:_="" ns3:_="">
     <xsd:import namespace="64be0a4d-3311-429d-90bd-b8f8a98a2612"/>
@@ -15031,6 +15025,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15041,23 +15041,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7962C7C6-1563-44DA-A4F9-B0C8B04A9566}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="64be0a4d-3311-429d-90bd-b8f8a98a2612"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="71fe8976-8fa5-4ae7-925c-3f33484c4e59"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B975C2-CA54-42AB-9376-238BCC154845}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15076,6 +15059,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7962C7C6-1563-44DA-A4F9-B0C8B04A9566}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="71fe8976-8fa5-4ae7-925c-3f33484c4e59"/>
+    <ds:schemaRef ds:uri="64be0a4d-3311-429d-90bd-b8f8a98a2612"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6651B7F8-C581-4C06-B93F-88C023FBB5C6}">
   <ds:schemaRefs>

</xml_diff>